<commit_message>
Roughing out the yaml format for data definitions
</commit_message>
<xml_diff>
--- a/devnotes/spreadsheet_mockup.xlsx
+++ b/devnotes/spreadsheet_mockup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/go/src/github.com/nryberg/data-garden/devnotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F4B1F1B-90F0-FE4C-92F8-492B35B83359}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827425EA-5E4D-D646-B5E9-861FB9B06BDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{FFA179E9-6F3A-4340-9405-CDB65755A148}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{FFA179E9-6F3A-4340-9405-CDB65755A148}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Customer</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Customer_Location</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C1E3ED-D303-5F45-9D94-C51079325F53}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -542,23 +545,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C38D130-444F-8C4C-BE72-EA2A8A128FE8}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -566,7 +572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -574,7 +580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -582,7 +588,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -590,7 +596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -598,7 +604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -615,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5F6701-2982-5247-8AD6-C64A4006C062}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>